<commit_message>
edycja pdf.py worksheet.write zmiana formatu wpisywania do arkusza z wspolrzednych na komorki
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -19,19 +19,19 @@
     <t>Zleceniodawca</t>
   </si>
   <si>
-    <t>wew2</t>
+    <t>cos xd</t>
   </si>
   <si>
     <t>Miejsce</t>
   </si>
   <si>
-    <t>s it</t>
+    <t>cos</t>
   </si>
   <si>
     <t>Nazwa</t>
   </si>
   <si>
-    <t xml:space="preserve">asfasb </t>
+    <t>cos xddd</t>
   </si>
 </sst>
 </file>
@@ -395,5 +395,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
utworzenie generacji danych do arkusza strona tytułowa oraz 1 zestaw tabel dla dwóch stron arkusza
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -14,24 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+  <si>
+    <t>Wojwódzki Szpital Zespolony</t>
+  </si>
+  <si>
+    <t>Orzeczenie Techniczne</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>xx/yy</t>
+  </si>
+  <si>
+    <t>Wystawione dnia xx/miesiac/zzzz</t>
+  </si>
   <si>
     <t>Zleceniodawca</t>
   </si>
   <si>
-    <t>cos xd</t>
-  </si>
-  <si>
-    <t>Miejsce</t>
-  </si>
-  <si>
-    <t>cos</t>
-  </si>
-  <si>
-    <t>Nazwa</t>
-  </si>
-  <si>
-    <t>cos xddd</t>
+    <t>SEK IT</t>
+  </si>
+  <si>
+    <t>Miejsce Użytkowania</t>
+  </si>
+  <si>
+    <t>Wew2</t>
+  </si>
+  <si>
+    <t>Nazwa Urzadzenia</t>
+  </si>
+  <si>
+    <t>drukarka</t>
   </si>
 </sst>
 </file>
@@ -363,34 +378,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
         <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodanie #cell definitions merge i bold
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>Wojwódzki Szpital Zespolony</t>
   </si>
@@ -34,27 +34,29 @@
     <t>Zleceniodawca</t>
   </si>
   <si>
-    <t>SEK IT</t>
+    <t>asd</t>
   </si>
   <si>
     <t>Miejsce Użytkowania</t>
   </si>
   <si>
-    <t>Wew2</t>
-  </si>
-  <si>
     <t>Nazwa Urzadzenia</t>
-  </si>
-  <si>
-    <t>drukarka</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -70,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,12 +80,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +414,10 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -421,13 +442,17 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J7" t="s">
@@ -435,34 +460,50 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
-        <v>9</v>
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="J9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
dodanie automatynczego wstawiania czasu "data"
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>Wojwódzki Szpital Zespolony</t>
   </si>
@@ -28,16 +28,19 @@
     <t>xx/yy</t>
   </si>
   <si>
-    <t>Wystawione dnia xx/miesiac/zzzz</t>
+    <t>Wystawione dnia 2022-10-27</t>
   </si>
   <si>
     <t>Zleceniodawca</t>
   </si>
   <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>Miejsce Użytkowania</t>
+  </si>
+  <si>
     <t>asd</t>
-  </si>
-  <si>
-    <t>Miejsce Użytkowania</t>
   </si>
   <si>
     <t>Nazwa Urzadzenia</t>
@@ -99,9 +102,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -399,29 +407,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="C1" t="s">
+    <row r="1" spans="1:13">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:13">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -441,68 +457,90 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J7" t="s">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J8" t="s">
-        <v>6</v>
-      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:13">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J9" t="s">
-        <v>6</v>
-      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="16">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J3:L3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
dodanie generacji końca arkusza
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Wojwódzki Szpital Zespolony</t>
   </si>
@@ -34,16 +34,31 @@
     <t>Zleceniodawca</t>
   </si>
   <si>
-    <t>as</t>
+    <t>ssdf</t>
   </si>
   <si>
     <t>Miejsce Użytkowania</t>
   </si>
   <si>
-    <t>asd</t>
+    <t>sadfsdg</t>
   </si>
   <si>
     <t>Nazwa Urzadzenia</t>
+  </si>
+  <si>
+    <t>dafsdf</t>
+  </si>
+  <si>
+    <t>Zespół Orzekający:</t>
+  </si>
+  <si>
+    <t>1 ................</t>
+  </si>
+  <si>
+    <t>2 ................</t>
+  </si>
+  <si>
+    <t>Zatwierdzam</t>
   </si>
 </sst>
 </file>
@@ -102,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -111,6 +126,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -407,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,7 +525,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -517,14 +535,50 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="M26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="H29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="H33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="22">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="J1:L1"/>
@@ -541,6 +595,12 @@
     <mergeCell ref="J8:M8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:M9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H33:I33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
prac ciag dalszy xD
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Wojwódzki Szpital Zespolony</t>
   </si>
@@ -49,13 +49,46 @@
     <t>dafsdf</t>
   </si>
   <si>
+    <t>Charakterystyka urządzenia</t>
+  </si>
+  <si>
+    <t>a) typ</t>
+  </si>
+  <si>
+    <t>c) rok produkcji</t>
+  </si>
+  <si>
+    <t>e) czas ekslpoatacji</t>
+  </si>
+  <si>
+    <t>g) wartość księgowa</t>
+  </si>
+  <si>
+    <t>b) nr fab.</t>
+  </si>
+  <si>
+    <t>d) nr inw.</t>
+  </si>
+  <si>
+    <t>f) producent</t>
+  </si>
+  <si>
+    <t>h) amortyzacja</t>
+  </si>
+  <si>
+    <t>Opis Stanu Technicznego</t>
+  </si>
+  <si>
+    <t>skdjhngvuioabgfuavbrqberuovb[qeriogbf[aerioavbio[erh[aerigbre0hfwqgbkoer</t>
+  </si>
+  <si>
     <t>Zespół Orzekający:</t>
   </si>
   <si>
-    <t>1 ................</t>
-  </si>
-  <si>
-    <t>2 ................</t>
+    <t>1 .........................</t>
+  </si>
+  <si>
+    <t>2 .........................</t>
   </si>
   <si>
     <t>Zatwierdzam</t>
@@ -126,7 +159,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -541,44 +574,198 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+    </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="F26" t="s">
-        <v>14</v>
+      <c r="E26" t="s">
+        <v>25</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="M26" t="s">
-        <v>14</v>
+      <c r="L26" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B29" s="4"/>
       <c r="H29" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="I29" s="4"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B33" s="4"/>
       <c r="H33" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="I33" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="44">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="J1:L1"/>
@@ -595,6 +782,28 @@
     <mergeCell ref="J8:M8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:M9"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F20"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="H18:M20"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A33:B33"/>

</xml_diff>

<commit_message>
prawie skonczony arkusz ustawione formatowanie i takie tam xD
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$33</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Wojwódzki Szpital Zespolony</t>
   </si>
@@ -34,19 +37,19 @@
     <t>Zleceniodawca</t>
   </si>
   <si>
-    <t>ssdf</t>
+    <t>Sekcja Informatyki i Telekomunikacji</t>
   </si>
   <si>
     <t>Miejsce Użytkowania</t>
   </si>
   <si>
-    <t>sadfsdg</t>
+    <t>Oddział Wew2</t>
   </si>
   <si>
     <t>Nazwa Urzadzenia</t>
   </si>
   <si>
-    <t>dafsdf</t>
+    <t>Drukarka Brother</t>
   </si>
   <si>
     <t>Charakterystyka urządzenia</t>
@@ -55,6 +58,9 @@
     <t>a) typ</t>
   </si>
   <si>
+    <t>MFC-7460DN</t>
+  </si>
+  <si>
     <t>c) rok produkcji</t>
   </si>
   <si>
@@ -67,19 +73,31 @@
     <t>b) nr fab.</t>
   </si>
   <si>
+    <t>CDN12345678</t>
+  </si>
+  <si>
     <t>d) nr inw.</t>
   </si>
   <si>
+    <t>102/14</t>
+  </si>
+  <si>
     <t>f) producent</t>
   </si>
   <si>
+    <t>Brother</t>
+  </si>
+  <si>
     <t>h) amortyzacja</t>
   </si>
   <si>
+    <t>100%</t>
+  </si>
+  <si>
     <t>Opis Stanu Technicznego</t>
   </si>
   <si>
-    <t>skdjhngvuioabgfuavbrqberuovb[qeriogbf[aerioavbio[erh[aerigbre0hfwqgbkoer</t>
+    <t>Drukarka po gwarancji. Uszkodzone elementy mechaniczne- 4 lat ciągłej pracy. Naprawa nieopłacalna.</t>
   </si>
   <si>
     <t>Zespół Orzekający:</t>
@@ -98,7 +116,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +126,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -150,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,6 +187,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -463,6 +493,15 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="C1" s="1" t="s">
@@ -513,22 +552,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="H7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
@@ -557,22 +596,22 @@
         <v>9</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
@@ -597,76 +636,124 @@
         <v>12</v>
       </c>
       <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="H12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="3"/>
+      <c r="J12" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="K12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L12" s="3"/>
+      <c r="M12" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3"/>
+      <c r="C13" s="4">
+        <v>2014</v>
+      </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E13" s="3"/>
+      <c r="F13" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="H13" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I13" s="3"/>
+      <c r="J13" s="4">
+        <v>2014</v>
+      </c>
       <c r="K13" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L13" s="3"/>
+      <c r="M13" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="3"/>
+      <c r="C14" s="4">
+        <v>8</v>
+      </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3"/>
+      <c r="F14" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="H14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I14" s="3"/>
+      <c r="J14" s="4">
+        <v>8</v>
+      </c>
       <c r="K14" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L14" s="3"/>
+      <c r="M14" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3"/>
+      <c r="C15" s="4">
+        <v>768.9</v>
+      </c>
       <c r="D15" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E15" s="3"/>
+      <c r="F15" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I15" s="3"/>
+      <c r="J15" s="4">
+        <v>768.9</v>
+      </c>
       <c r="K15" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L15" s="3"/>
+      <c r="M15" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -674,7 +761,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -684,7 +771,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -692,7 +779,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -729,40 +816,40 @@
       <c r="M20" s="3"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="4"/>
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="5"/>
       <c r="E26" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="5"/>
       <c r="L26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="H29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I29" s="4"/>
+      <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="5"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="H33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I33" s="4"/>
+      <c r="A33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="H33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -811,7 +898,8 @@
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="H33:I33"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dokończenie generacji arkusza i drobne poprawki -> podjecie dzialan do stworzenia bazy danych, kont uzytkownikow.
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -17,9 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
-  <si>
-    <t>Wojwódzki Szpital Zespolony</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+  <si>
+    <t>Wojewódzki Szpital Zespolony</t>
   </si>
   <si>
     <t>Orzeczenie Techniczne</t>
@@ -28,22 +28,25 @@
     <t>nr</t>
   </si>
   <si>
+    <t>178/2022</t>
+  </si>
+  <si>
+    <t>Wystawione dnia 2022-10-27</t>
+  </si>
+  <si>
     <t>xx/yy</t>
   </si>
   <si>
-    <t>Wystawione dnia 2022-10-27</t>
-  </si>
-  <si>
     <t>Zleceniodawca</t>
   </si>
   <si>
-    <t>Sekcja Informatyki i Telekomunikacji</t>
+    <t>Sekcja Informatyki</t>
   </si>
   <si>
     <t>Miejsce Użytkowania</t>
   </si>
   <si>
-    <t>Oddział Wew2</t>
+    <t>Oddział Wew 2</t>
   </si>
   <si>
     <t>Nazwa Urzadzenia</t>
@@ -58,13 +61,13 @@
     <t>a) typ</t>
   </si>
   <si>
-    <t>MFC-7460DN</t>
+    <t>MFC - 7460DN</t>
   </si>
   <si>
     <t>c) rok produkcji</t>
   </si>
   <si>
-    <t>e) czas ekslpoatacji</t>
+    <t>e) czas eksploatacji</t>
   </si>
   <si>
     <t>g) wartość księgowa</t>
@@ -73,13 +76,13 @@
     <t>b) nr fab.</t>
   </si>
   <si>
-    <t>CDN12345678</t>
+    <t>CDN123456</t>
   </si>
   <si>
     <t>d) nr inw.</t>
   </si>
   <si>
-    <t>102/14</t>
+    <t>123/14</t>
   </si>
   <si>
     <t>f) producent</t>
@@ -97,7 +100,13 @@
     <t>Opis Stanu Technicznego</t>
   </si>
   <si>
-    <t>Drukarka po gwarancji. Uszkodzone elementy mechaniczne- 4 lat ciągłej pracy. Naprawa nieopłacalna.</t>
+    <t>Drukarka nie zdatna do użytku uszkodzony utrwalacz</t>
+  </si>
+  <si>
+    <t>Uwagi i wnioski</t>
+  </si>
+  <si>
+    <t>Proszę o zgodę na skasowanie ww. sprzętu</t>
   </si>
   <si>
     <t>Zespół Orzekający:</t>
@@ -177,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,6 +198,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -541,7 +553,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
@@ -549,21 +561,21 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="H7" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -571,43 +583,43 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="H8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="J8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="H9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -615,7 +627,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -623,7 +635,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -633,127 +645,127 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4">
         <v>2014</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="4">
         <v>2014</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4">
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="4">
         <v>8</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4">
-        <v>768.9</v>
+        <v>678.67</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="4">
-        <v>768.9</v>
+        <v>678.67</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -761,7 +773,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -771,7 +783,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -779,7 +791,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -815,44 +827,80 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+    </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="5"/>
+      <c r="A26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="6"/>
       <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26" s="5"/>
+      <c r="I26" s="6"/>
       <c r="L26" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="H29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="5"/>
+      <c r="A29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="6"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="H33" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I33" s="5"/>
+      <c r="A33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="H33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="48">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="J1:L1"/>
@@ -891,6 +939,10 @@
     <mergeCell ref="A18:F20"/>
     <mergeCell ref="H17:M17"/>
     <mergeCell ref="H18:M20"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H23:M23"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A33:B33"/>

</xml_diff>

<commit_message>
kosmetyka formularz i uspójninie nazw plików
</commit_message>
<xml_diff>
--- a/Orzeczenie_Tech.xlsx
+++ b/Orzeczenie_Tech.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Wojewódzki Szpital Zespolony</t>
   </si>
@@ -31,24 +31,18 @@
     <t>178/2022</t>
   </si>
   <si>
-    <t>Wystawione dnia 2022-10-27</t>
-  </si>
-  <si>
-    <t>xx/yy</t>
+    <t>Wystawione dnia 2022-10-28</t>
   </si>
   <si>
     <t>Zleceniodawca</t>
   </si>
   <si>
-    <t>Sekcja Informatyki</t>
+    <t>Sekcja Informatyki i Telekomunikacji</t>
   </si>
   <si>
     <t>Miejsce Użytkowania</t>
   </si>
   <si>
-    <t>Oddział Wew 2</t>
-  </si>
-  <si>
     <t>Nazwa Urzadzenia</t>
   </si>
   <si>
@@ -61,7 +55,7 @@
     <t>a) typ</t>
   </si>
   <si>
-    <t>MFC - 7460DN</t>
+    <t>MFC-7460DN</t>
   </si>
   <si>
     <t>c) rok produkcji</t>
@@ -76,7 +70,7 @@
     <t>b) nr fab.</t>
   </si>
   <si>
-    <t>CDN123456</t>
+    <t>CDN12345678</t>
   </si>
   <si>
     <t>d) nr inw.</t>
@@ -100,7 +94,7 @@
     <t>Opis Stanu Technicznego</t>
   </si>
   <si>
-    <t>Drukarka nie zdatna do użytku uszkodzony utrwalacz</t>
+    <t>afhwrvtrhtjustrhshsryjrsgasdcb habvoerbguearigbpuaeiogbriuaerfpoarht[awgh[awrg[awerbhvoiarhgaergh[0aer9gh[qa</t>
   </si>
   <si>
     <t>Uwagi i wnioski</t>
@@ -186,13 +180,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -540,371 +537,379 @@
       <c r="L3" s="2"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="H7" s="3" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="3" t="s">
+      <c r="I8" s="4"/>
+      <c r="J8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="5" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="H8" s="3" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="H9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="5" t="s">
+      <c r="I9" s="4"/>
+      <c r="J9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="3" t="s">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="H9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="4" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="3" t="s">
+      <c r="I12" s="4"/>
+      <c r="J12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="3" t="s">
+      <c r="K12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5">
+        <v>2014</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5">
+        <v>2014</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="3" t="s">
+      <c r="I14" s="4"/>
+      <c r="J14" s="5">
+        <v>8</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4">
-        <v>2014</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5">
+        <v>123.123</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="4">
-        <v>2014</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="I15" s="4"/>
+      <c r="J15" s="5">
+        <v>123.123</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4" t="s">
+      <c r="L15" s="4"/>
+      <c r="M15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="4">
-        <v>8</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4">
-        <v>678.67</v>
-      </c>
-      <c r="D15" s="3" t="s">
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4">
-        <v>678.67</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="4" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="3" t="s">
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="H17" s="3" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="H22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="3" t="s">
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="H18" s="3" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="H23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="3" t="s">
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="H22" s="3" t="s">
+      <c r="B26" s="7"/>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="3" t="s">
+      <c r="I26" s="7"/>
+      <c r="L26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="H23" s="3" t="s">
+      <c r="B29" s="7"/>
+      <c r="H29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="6" t="s">
+      <c r="I29" s="7"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="E26" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="6" t="s">
+      <c r="B33" s="7"/>
+      <c r="H33" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I26" s="6"/>
-      <c r="L26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="H29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="H33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I33" s="6"/>
+      <c r="I33" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="50">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C5:F5"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J5:M5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A8:B8"/>

</xml_diff>